<commit_message>
Update sales.xlsx from Streamlit app
</commit_message>
<xml_diff>
--- a/sales.xlsx
+++ b/sales.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,10 +515,8 @@
           <t>2025-09-09 16:34:44</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>5421</t>
-        </is>
+      <c r="B3" t="n">
+        <v>5421</v>
       </c>
       <c r="C3" t="n">
         <v>6698</v>
@@ -538,6 +536,44 @@
       <c r="H3" t="inlineStr">
         <is>
           <t>Return</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-09-11 06:08:50</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1220</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>6698</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>199</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ALLAN</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CHRIS</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Sale</t>
         </is>
       </c>
     </row>

</xml_diff>